<commit_message>
updated with paper's series of counterexamples.
</commit_message>
<xml_diff>
--- a/axioms_counter_examples.xlsx
+++ b/axioms_counter_examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/n7176546_qut_edu_au/Documents/phd/mypapers/CAiSE2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="568" documentId="8_{3651E306-56F1-49A5-AB53-C60922551D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD7D5401-D3E8-4276-9938-7E82B96BA272}"/>
+  <xr:revisionPtr revIDLastSave="627" documentId="8_{3651E306-56F1-49A5-AB53-C60922551D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41F04625-F828-4919-99DC-FA6B48C86D91}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8AB40EBB-997B-41B2-9ACE-A729633260DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{8AB40EBB-997B-41B2-9ACE-A729633260DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Axiom 3" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="80">
   <si>
     <t>log_1</t>
   </si>
@@ -139,9 +139,6 @@
     <t>* is one this technique min? Given the edit distance, the worst distance is likely more… as for each event we could induce a cost of at least one … meaning min at least 4</t>
   </si>
   <si>
-    <t>In order to have a possiblity to adhere to axiom 9, measures should the same for each log. (conducted ten runs as unintented behaviour was observed)</t>
-  </si>
-  <si>
     <t xml:space="preserve">gprec_D = </t>
   </si>
   <si>
@@ -263,6 +260,27 @@
   </si>
   <si>
     <t xml:space="preserve"> using all process attributes</t>
+  </si>
+  <si>
+    <t>In order to have a possiblity to adhere to axiom 9, measures should be the same for each log. (conducted ten runs as unintented behaviour was observed)</t>
+  </si>
+  <si>
+    <t>model_6</t>
+  </si>
+  <si>
+    <t>add model_6 is all true</t>
+  </si>
+  <si>
+    <t>ax_3_model_5</t>
+  </si>
+  <si>
+    <t>ax_3_model_4</t>
+  </si>
+  <si>
+    <t>ax_3_model_1</t>
+  </si>
+  <si>
+    <t>using log for axiom 3</t>
   </si>
 </sst>
 </file>
@@ -663,15 +681,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B49AACE-69E8-4DCD-942E-1B8581E5BA66}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -687,11 +705,14 @@
       <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -710,11 +731,11 @@
       <c r="F2">
         <v>0.97699999999999998</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -733,11 +754,11 @@
       <c r="F3">
         <v>0.97699999999999998</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -756,31 +777,34 @@
       <c r="F4">
         <v>0.48799999999999999</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -788,7 +812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -796,7 +820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -814,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CC6BA3-3425-419C-AF32-CA4969E751E1}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -917,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C46C642-8D29-4653-8F48-0EB61CE03BA9}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1032,16 +1056,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537A8F8B-B6E1-4C72-A72D-908CA78D7D34}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
@@ -1054,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1075,28 +1100,28 @@
         <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
         <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" t="s">
-        <v>59</v>
       </c>
       <c r="Q1" t="s">
         <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T1" t="s">
         <v>2</v>
@@ -1119,7 +1144,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>0.81299999999999994</v>
@@ -1140,7 +1165,7 @@
         <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K2">
         <v>0.75700000000000001</v>
@@ -1161,7 +1186,7 @@
         <v>27</v>
       </c>
       <c r="S2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T2">
         <v>0.58499999999999996</v>
@@ -1184,7 +1209,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>0.82299999999999995</v>
@@ -1205,7 +1230,7 @@
         <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K3">
         <v>0.75800000000000001</v>
@@ -1226,7 +1251,7 @@
         <v>27</v>
       </c>
       <c r="S3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T3">
         <v>0.58099999999999996</v>
@@ -1249,7 +1274,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>0.77400000000000002</v>
@@ -1270,7 +1295,7 @@
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4">
         <v>0.75800000000000001</v>
@@ -1291,7 +1316,7 @@
         <v>27</v>
       </c>
       <c r="S4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T4">
         <v>0.58499999999999996</v>
@@ -1314,7 +1339,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0.82299999999999995</v>
@@ -1335,7 +1360,7 @@
         <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5">
         <v>0.75800000000000001</v>
@@ -1356,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="S5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T5">
         <v>0.58099999999999996</v>
@@ -1379,7 +1404,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>0.82299999999999995</v>
@@ -1400,7 +1425,7 @@
         <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6">
         <v>0.75800000000000001</v>
@@ -1421,7 +1446,7 @@
         <v>27</v>
       </c>
       <c r="S6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T6">
         <v>0.58499999999999996</v>
@@ -1444,7 +1469,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <v>0.81299999999999994</v>
@@ -1465,7 +1490,7 @@
         <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K7">
         <v>0.75700000000000001</v>
@@ -1486,7 +1511,7 @@
         <v>27</v>
       </c>
       <c r="S7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T7">
         <v>0.58499999999999996</v>
@@ -1509,7 +1534,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>0.81299999999999994</v>
@@ -1530,7 +1555,7 @@
         <v>27</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K8">
         <v>0.75800000000000001</v>
@@ -1551,7 +1576,7 @@
         <v>27</v>
       </c>
       <c r="S8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T8">
         <v>0.58199999999999996</v>
@@ -1574,7 +1599,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>0.82299999999999995</v>
@@ -1595,7 +1620,7 @@
         <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K9">
         <v>0.75700000000000001</v>
@@ -1616,7 +1641,7 @@
         <v>27</v>
       </c>
       <c r="S9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T9">
         <v>0.58499999999999996</v>
@@ -1639,7 +1664,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>0.82299999999999995</v>
@@ -1660,7 +1685,7 @@
         <v>27</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K10">
         <v>0.75800000000000001</v>
@@ -1681,7 +1706,7 @@
         <v>27</v>
       </c>
       <c r="S10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T10">
         <v>0.58499999999999996</v>
@@ -1704,7 +1729,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>0.82299999999999995</v>
@@ -1725,7 +1750,7 @@
         <v>27</v>
       </c>
       <c r="J11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K11">
         <v>0.75800000000000001</v>
@@ -1746,7 +1771,7 @@
         <v>27</v>
       </c>
       <c r="S11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T11">
         <v>0.58499999999999996</v>
@@ -1769,36 +1794,36 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" t="s">
+        <v>59</v>
+      </c>
+      <c r="U12" t="s">
         <v>53</v>
-      </c>
-      <c r="L12" t="s">
-        <v>60</v>
-      </c>
-      <c r="U12" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T14" t="s">
+        <v>57</v>
+      </c>
+      <c r="U14" t="s">
+        <v>56</v>
+      </c>
+      <c r="V14" t="s">
+        <v>55</v>
+      </c>
+      <c r="W14" t="s">
+        <v>54</v>
+      </c>
+      <c r="X14" t="s">
         <v>58</v>
-      </c>
-      <c r="U14" t="s">
-        <v>57</v>
-      </c>
-      <c r="V14" t="s">
-        <v>56</v>
-      </c>
-      <c r="W14" t="s">
-        <v>55</v>
-      </c>
-      <c r="X14" t="s">
-        <v>59</v>
       </c>
       <c r="Z14" t="s">
         <v>17</v>
@@ -1809,7 +1834,7 @@
         <v>6</v>
       </c>
       <c r="S15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T15">
         <v>0.69399999999999995</v>
@@ -1832,10 +1857,10 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T16">
         <v>0.69499999999999995</v>
@@ -1858,7 +1883,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T17">
         <v>0.69499999999999995</v>
@@ -1881,7 +1906,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T18">
         <v>0.69399999999999995</v>
@@ -1904,13 +1929,28 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
-        <v>34</v>
+      <c r="I19" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K19" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N19" t="s">
+        <v>17</v>
       </c>
       <c r="S19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T19">
         <v>0.69499999999999995</v>
@@ -1932,8 +1972,23 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20">
+        <v>0.95</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="S20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T20">
         <v>0.69499999999999995</v>
@@ -1955,8 +2010,23 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="S21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T21">
         <v>0.69499999999999995</v>
@@ -1978,8 +2048,23 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="S22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T22">
         <v>0.69399999999999995</v>
@@ -2001,8 +2086,23 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="K23">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="L23">
+        <v>0.9</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="S23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T23">
         <v>0.69399999999999995</v>
@@ -2024,8 +2124,23 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="S24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T24">
         <v>0.69399999999999995</v>
@@ -2047,8 +2162,101 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="K25">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="L25">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="U25" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="K26">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="L26">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>43</v>
+      </c>
+      <c r="J28">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>0.9</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0.9</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2061,7 +2269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC1133B-0119-4605-A3D0-8F060F37A946}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -2074,7 +2282,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2092,7 +2300,7 @@
         <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
@@ -2112,7 +2320,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -2130,7 +2338,7 @@
         <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
         <v>21</v>
@@ -2150,7 +2358,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -2168,7 +2376,7 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>
@@ -2188,7 +2396,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2206,7 +2414,7 @@
         <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
@@ -2226,7 +2434,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2244,7 +2452,7 @@
         <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
         <v>21</v>
@@ -2264,7 +2472,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -2282,7 +2490,7 @@
         <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
@@ -2302,7 +2510,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -2320,7 +2528,7 @@
         <v>23</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
         <v>21</v>
@@ -2340,7 +2548,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -2358,7 +2566,7 @@
         <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K8" t="s">
         <v>21</v>
@@ -2378,7 +2586,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -2396,7 +2604,7 @@
         <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K9" t="s">
         <v>21</v>
@@ -2416,7 +2624,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
@@ -2434,7 +2642,7 @@
         <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K10" t="s">
         <v>21</v>
@@ -2454,7 +2662,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -2472,7 +2680,7 @@
         <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K11" t="s">
         <v>21</v>
@@ -2492,15 +2700,15 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" t="s">
         <v>72</v>
-      </c>
-      <c r="M12" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -2513,10 +2721,10 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2529,15 +2737,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C1973C-B9E9-4C75-A656-D5220DCE9D6A}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2552,7 +2760,7 @@
         <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -2569,7 +2777,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>0.95399999999999996</v>
@@ -2584,7 +2792,7 @@
         <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2">
         <v>0.92900000000000005</v>
@@ -2601,7 +2809,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>0.97399999999999998</v>
@@ -2613,10 +2821,10 @@
         <v>0.97399999999999998</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3">
         <v>0.92900000000000005</v>
@@ -2633,7 +2841,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2645,10 +2853,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4">
         <v>0.92900000000000005</v>
@@ -2665,7 +2873,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0.93200000000000005</v>
@@ -2680,7 +2888,7 @@
         <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5">
         <v>0.92900000000000005</v>
@@ -2697,7 +2905,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>0.95899999999999996</v>
@@ -2709,10 +2917,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6">
         <v>0.92900000000000005</v>
@@ -2729,7 +2937,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2744,7 +2952,7 @@
         <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7">
         <v>0.92900000000000005</v>
@@ -2761,7 +2969,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>0.97399999999999998</v>
@@ -2776,7 +2984,7 @@
         <v>23</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8">
         <v>0.92900000000000005</v>
@@ -2793,7 +3001,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2808,7 +3016,7 @@
         <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9">
         <v>0.92900000000000005</v>
@@ -2820,12 +3028,12 @@
         <v>0.9</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2837,10 +3045,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10">
         <v>0.92900000000000005</v>
@@ -2857,7 +3065,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>0.93799999999999994</v>
@@ -2869,10 +3077,10 @@
         <v>0.98599999999999999</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J11">
         <v>0.92900000000000005</v>
@@ -2889,28 +3097,28 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
         <v>47</v>
-      </c>
-      <c r="J12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding some testing for unpublished measures.
Their adherence in comparison to the existing work is similar.
</commit_message>
<xml_diff>
--- a/axioms_counter_examples.xlsx
+++ b/axioms_counter_examples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/n7176546_qut_edu_au/Documents/phd/mypapers/CAiSE2023/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/n7176546_qut_edu_au/Documents/phd/mypapers/CAiSE2023/data/data-aware conformance/data-aware-propositions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="627" documentId="8_{3651E306-56F1-49A5-AB53-C60922551D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41F04625-F828-4919-99DC-FA6B48C86D91}"/>
+  <xr:revisionPtr revIDLastSave="820" documentId="8_{3651E306-56F1-49A5-AB53-C60922551D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E890984B-6E84-44D8-8634-78C7F7D4E11E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{8AB40EBB-997B-41B2-9ACE-A729633260DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{8AB40EBB-997B-41B2-9ACE-A729633260DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Axiom 3" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="92">
   <si>
     <t>log_1</t>
   </si>
@@ -281,6 +281,42 @@
   </si>
   <si>
     <t>using log for axiom 3</t>
+  </si>
+  <si>
+    <t>grec_E</t>
+  </si>
+  <si>
+    <t>grec_E =</t>
+  </si>
+  <si>
+    <t>0.461**</t>
+  </si>
+  <si>
+    <t>** for ten unique runs two different values were observed, but the std was 1e-15 for this set. Likely a precision collapse.</t>
+  </si>
+  <si>
+    <t>Previously proposed 'reasoning_recall' technique for CAiSE2023</t>
+  </si>
+  <si>
+    <t>1**</t>
+  </si>
+  <si>
+    <t>** is 1.0 the maximun possible result for this unpublished technique? No the 'max' or worst case of this technique is 0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gprec_F = </t>
+  </si>
+  <si>
+    <t>Previously proposed 'reasoning_precision' technique for CAiSE2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gprec_F </t>
+  </si>
+  <si>
+    <t>Numerical Collapse caused a std of  at least 2e-15</t>
+  </si>
+  <si>
+    <t>gprec_F</t>
   </si>
 </sst>
 </file>
@@ -378,10 +414,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -681,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B49AACE-69E8-4DCD-942E-1B8581E5BA66}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,48 +816,84 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>30</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -836,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CC6BA3-3425-419C-AF32-CA4969E751E1}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,48 +956,72 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -939,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C46C642-8D29-4653-8F48-0EB61CE03BA9}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,6 +1104,23 @@
         <v>27</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
@@ -1047,6 +1156,14 @@
       </c>
       <c r="B14" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1056,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537A8F8B-B6E1-4C72-A72D-908CA78D7D34}">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,6 +2089,12 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
       <c r="I20" t="s">
         <v>35</v>
       </c>
@@ -2257,6 +2380,264 @@
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K31" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>89</v>
+      </c>
+      <c r="J33" t="s">
+        <v>2</v>
+      </c>
+      <c r="K33" t="s">
+        <v>3</v>
+      </c>
+      <c r="L33" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" t="s">
+        <v>5</v>
+      </c>
+      <c r="N33" t="s">
+        <v>16</v>
+      </c>
+      <c r="P33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>35</v>
+      </c>
+      <c r="J34">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K34">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L34">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M34">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>36</v>
+      </c>
+      <c r="J35">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K35">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L35">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M35">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K36">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L36">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M36">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K37">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L37">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M37">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K38">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L38">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M38">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>40</v>
+      </c>
+      <c r="J39">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K39">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L39">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M39">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>41</v>
+      </c>
+      <c r="J40">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K40">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L40">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M40">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K41">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L41">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M41">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K42">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L42">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M42">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>44</v>
+      </c>
+      <c r="J43">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K43">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L43">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="M43">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2267,10 +2648,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC1133B-0119-4605-A3D0-8F060F37A946}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2719,12 +3100,241 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
+      </c>
+      <c r="K17" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" t="s">
+        <v>5</v>
+      </c>
+      <c r="R17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N18">
+        <v>0.5</v>
+      </c>
+      <c r="O18">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N19">
+        <v>0.5</v>
+      </c>
+      <c r="O19">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>62</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N20">
+        <v>0.5</v>
+      </c>
+      <c r="O20">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N21">
+        <v>0.5</v>
+      </c>
+      <c r="O21">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>64</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N22">
+        <v>0.5</v>
+      </c>
+      <c r="O22">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>65</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N23">
+        <v>0.5</v>
+      </c>
+      <c r="O23">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N24">
+        <v>0.5</v>
+      </c>
+      <c r="O24">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N25">
+        <v>0.5</v>
+      </c>
+      <c r="O25">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N26">
+        <v>0.5</v>
+      </c>
+      <c r="O26">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>69</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="N27">
+        <v>0.5</v>
+      </c>
+      <c r="O27">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2735,10 +3345,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C1973C-B9E9-4C75-A656-D5220DCE9D6A}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3113,12 +3723,212 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>